<commit_message>
added strats and folders cleansing
Removed the PyCharm ".idea" folder from github
Removed the "Data" folder  as no data should be uploadedon github
All orangeModels have been removed, and only the relevant ones will be added in an upcoming commit
strategy 50pipsADay has been renamed to 7amUK
only 3 strategies have been kept: swing, macdRsi, 7amUK
</commit_message>
<xml_diff>
--- a/scripts/backtestStrategy.xlsx
+++ b/scripts/backtestStrategy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbp13/OneDrive/GitHub/Trading-Predictions-Framework/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C039580-C1F8-2545-AA84-1D73A109CB61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C104C3B5-BACE-B64C-B4B9-72A680DDAB4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{4B0CB58C-FB54-460E-ACA1-EF7D92DFC0C7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{4B0CB58C-FB54-460E-ACA1-EF7D92DFC0C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="11" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Actions!$A$1:$P$73</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ActionsMap!$A$1:$L$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ActionsMap!$A$1:$M$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Maps!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="76">
   <si>
     <t>Buying Signal</t>
   </si>
@@ -396,6 +396,13 @@
 3) opening (0,1,2)
 4) closing (0,1,2)
 5) TPSL (0,1,2,3)</t>
+  </si>
+  <si>
+    <t>hold</t>
+  </si>
+  <si>
+    <t>signalLabel
+(signal variable for machine learning)</t>
   </si>
 </sst>
 </file>
@@ -1109,12 +1116,12 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
       <selection activeCell="I11" sqref="I11"/>
       <selection pane="topRight" activeCell="I11" sqref="I11"/>
       <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5818,11 +5825,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8328D5CD-8CF1-BC46-8606-E898FDD50A7C}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5834,10 +5841,10 @@
     <col min="8" max="8" width="19.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="24.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="1" customWidth="1"/>
-    <col min="11" max="12" width="16.6640625" customWidth="1"/>
+    <col min="11" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="160" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="160" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -5874,26 +5881,29 @@
       <c r="L1" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" s="1">
         <f t="shared" ref="F2:F29" si="0">80000+_xlfn.NUMBERVALUE(B2&amp;C2&amp;D2&amp;E2)</f>
-        <v>80000</v>
+        <v>81010</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
@@ -5902,76 +5912,82 @@
         <v>0</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" si="0"/>
-        <v>80100</v>
+        <v>82020</v>
       </c>
       <c r="G3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>80110</v>
+        <v>80000</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -5983,57 +5999,63 @@
         <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>80200</v>
+        <v>80110</v>
       </c>
       <c r="G5" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>74</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="M5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -6045,11 +6067,11 @@
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>81010</v>
+        <v>81011</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -6058,21 +6080,24 @@
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="L6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -6084,11 +6109,11 @@
         <v>1</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>81011</v>
+        <v>81012</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -6097,21 +6122,24 @@
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -6123,11 +6151,11 @@
         <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>81012</v>
+        <v>81013</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -6135,38 +6163,41 @@
       <c r="H8" s="1">
         <v>0</v>
       </c>
-      <c r="I8" s="1">
-        <v>4</v>
+      <c r="I8" s="22">
+        <v>5</v>
       </c>
       <c r="J8" s="1">
         <v>0</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K8" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="M8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>81013</v>
+        <v>82021</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -6174,155 +6205,167 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="I9" s="22">
-        <v>5</v>
+      <c r="I9" s="1">
+        <v>3</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
       </c>
-      <c r="K9" s="20">
-        <v>0</v>
-      </c>
-      <c r="L9" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K9" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" t="s">
+        <v>74</v>
+      </c>
+      <c r="M9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>81100</v>
+        <v>82022</v>
       </c>
       <c r="G10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J10" s="1">
         <v>0</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>81111</v>
+        <v>82023</v>
       </c>
       <c r="G11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="I11" s="22">
+        <v>5</v>
       </c>
       <c r="J11" s="1">
         <v>0</v>
       </c>
-      <c r="K11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K11" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>81112</v>
+        <v>82200</v>
       </c>
       <c r="G12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="L12" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>81113</v>
+        <v>82120</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -6330,8 +6373,8 @@
       <c r="H13" s="1">
         <v>1</v>
       </c>
-      <c r="I13" s="22">
-        <v>5</v>
+      <c r="I13" s="1">
+        <v>2</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
@@ -6339,214 +6382,232 @@
       <c r="K13" t="s">
         <v>27</v>
       </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>81210</v>
+        <v>80100</v>
       </c>
       <c r="G14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1">
         <v>1</v>
       </c>
       <c r="I14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="1">
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="M14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>81211</v>
+        <v>81100</v>
       </c>
       <c r="G15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J15" s="1">
         <v>0</v>
       </c>
-      <c r="K15">
-        <v>0</v>
+      <c r="K15" t="s">
+        <v>27</v>
       </c>
       <c r="L15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="M15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>81212</v>
+        <v>81111</v>
       </c>
       <c r="G16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="1">
         <v>1</v>
       </c>
       <c r="I16" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J16" s="1">
         <v>0</v>
       </c>
-      <c r="K16">
-        <v>0</v>
+      <c r="K16" t="s">
+        <v>27</v>
       </c>
       <c r="L16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="M16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>81213</v>
+        <v>81112</v>
       </c>
       <c r="G17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" s="1">
         <v>1</v>
       </c>
-      <c r="I17" s="22">
-        <v>5</v>
+      <c r="I17" s="1">
+        <v>4</v>
       </c>
       <c r="J17" s="1">
         <v>0</v>
       </c>
-      <c r="K17">
-        <v>0</v>
+      <c r="K17" t="s">
+        <v>27</v>
       </c>
       <c r="L17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="M17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>82020</v>
+        <v>81113</v>
       </c>
       <c r="G18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="I18" s="22">
+        <v>5</v>
       </c>
       <c r="J18" s="1">
         <v>0</v>
       </c>
-      <c r="K18">
-        <v>0</v>
+      <c r="K18" t="s">
+        <v>27</v>
       </c>
       <c r="L18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="M18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
       </c>
       <c r="C19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
@@ -6556,13 +6617,13 @@
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>82021</v>
+        <v>82121</v>
       </c>
       <c r="G19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="1">
         <v>3</v>
@@ -6570,22 +6631,25 @@
       <c r="J19" s="1">
         <v>0</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K19" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" t="s">
+        <v>74</v>
+      </c>
+      <c r="M19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B20" s="1">
         <v>2</v>
       </c>
       <c r="C20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
@@ -6595,13 +6659,13 @@
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>82022</v>
+        <v>82122</v>
       </c>
       <c r="G20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="1">
         <v>4</v>
@@ -6609,22 +6673,25 @@
       <c r="J20" s="1">
         <v>0</v>
       </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K20" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" t="s">
+        <v>74</v>
+      </c>
+      <c r="M20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1">
         <v>2</v>
       </c>
       <c r="C21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
@@ -6634,13 +6701,13 @@
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>82023</v>
+        <v>82123</v>
       </c>
       <c r="G21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="22">
         <v>5</v>
@@ -6648,209 +6715,227 @@
       <c r="J21" s="1">
         <v>0</v>
       </c>
-      <c r="K21" s="20">
-        <v>0</v>
-      </c>
-      <c r="L21" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K21" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" t="s">
+        <v>74</v>
+      </c>
+      <c r="M21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>82120</v>
+        <v>81210</v>
       </c>
       <c r="G22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="1">
         <v>1</v>
       </c>
       <c r="I22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J22" s="1">
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="M22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>82121</v>
+        <v>80200</v>
       </c>
       <c r="G23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23" s="1">
         <v>1</v>
       </c>
       <c r="I23" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J23" s="1">
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>27</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="L23" t="s">
+        <v>29</v>
+      </c>
+      <c r="M23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>82122</v>
+        <v>81211</v>
       </c>
       <c r="G24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" s="1">
         <v>1</v>
       </c>
       <c r="I24" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J24" s="1">
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>27</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="L24" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>82123</v>
+        <v>81212</v>
       </c>
       <c r="G25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" s="1">
         <v>1</v>
       </c>
-      <c r="I25" s="22">
-        <v>5</v>
+      <c r="I25" s="1">
+        <v>4</v>
       </c>
       <c r="J25" s="1">
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>27</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="L25" t="s">
+        <v>29</v>
+      </c>
+      <c r="M25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="0"/>
-        <v>82200</v>
+        <v>81213</v>
       </c>
       <c r="G26" s="1">
         <v>2</v>
       </c>
       <c r="H26" s="1">
-        <v>2</v>
-      </c>
-      <c r="I26" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I26" s="22">
+        <v>5</v>
       </c>
       <c r="J26" s="1">
         <v>0</v>
       </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K26" t="s">
+        <v>74</v>
+      </c>
+      <c r="L26" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
@@ -6882,14 +6967,17 @@
       <c r="J27" s="1">
         <v>0</v>
       </c>
-      <c r="K27">
-        <v>0</v>
+      <c r="K27" t="s">
+        <v>74</v>
       </c>
       <c r="L27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
@@ -6921,14 +7009,17 @@
       <c r="J28" s="1">
         <v>0</v>
       </c>
-      <c r="K28">
-        <v>0</v>
+      <c r="K28" t="s">
+        <v>74</v>
       </c>
       <c r="L28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
@@ -6960,17 +7051,20 @@
       <c r="J29" s="1">
         <v>0</v>
       </c>
-      <c r="K29">
-        <v>0</v>
+      <c r="K29" t="s">
+        <v>74</v>
       </c>
       <c r="L29" t="s">
         <v>29</v>
       </c>
+      <c r="M29" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L28" xr:uid="{86103D8D-BDA0-A344-8717-55E245B8267A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L29">
-      <sortCondition ref="F1:F29"/>
+  <autoFilter ref="A1:M29" xr:uid="{AC4ECC62-B3FC-A849-AB8C-A63C8C141A33}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M29">
+      <sortCondition ref="M1:M29"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added quickModelling.py script + cleansing
this script will allow to skip manual steps in Knime and Orange to calculate variables and estimate a prediction score with these variables
</commit_message>
<xml_diff>
--- a/scripts/backtestStrategy.xlsx
+++ b/scripts/backtestStrategy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbp13/OneDrive/GitHub/Trading-Predictions-Framework/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xau\OneDrive\GitHub\Trading-Predictions-Framework\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C104C3B5-BACE-B64C-B4B9-72A680DDAB4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{C104C3B5-BACE-B64C-B4B9-72A680DDAB4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6B0D149F-A7F4-4DF7-A53E-48EC6A04ABFC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{4B0CB58C-FB54-460E-ACA1-EF7D92DFC0C7}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" activeTab="1" xr2:uid="{4B0CB58C-FB54-460E-ACA1-EF7D92DFC0C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="11" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ActionsMap!$A$1:$M$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Maps!$A$1:$L$1</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1116,31 +1118,31 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="I11" sqref="I11"/>
       <selection pane="topRight" activeCell="I11" sqref="I11"/>
       <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
-      <selection pane="bottomRight" activeCell="J75" sqref="J75"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="41" customWidth="1"/>
-    <col min="2" max="4" width="12.83203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="28" customWidth="1"/>
-    <col min="9" max="9" width="23.1640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="41" customWidth="1"/>
+    <col min="2" max="4" width="12.77734375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.109375" style="38" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="28" customWidth="1"/>
+    <col min="9" max="9" width="23.109375" style="28" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" style="30" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" style="31" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="32"/>
+    <col min="12" max="13" width="10.77734375" style="32"/>
     <col min="14" max="15" width="9" style="32" customWidth="1"/>
-    <col min="16" max="16" width="5.5" style="32" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="1"/>
+    <col min="16" max="16" width="5.44140625" style="32" customWidth="1"/>
+    <col min="17" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" ht="89" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="89.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
         <v>4</v>
       </c>
@@ -1190,7 +1192,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
@@ -1268,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
         <v>5</v>
       </c>
@@ -1331,7 +1333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
         <v>5</v>
       </c>
@@ -1394,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>5</v>
       </c>
@@ -1457,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
         <v>5</v>
       </c>
@@ -1520,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>5</v>
       </c>
@@ -1583,7 +1585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
         <v>5</v>
       </c>
@@ -1646,7 +1648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
         <v>5</v>
       </c>
@@ -1709,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="39" t="s">
         <v>6</v>
       </c>
@@ -1772,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="39" t="s">
         <v>6</v>
       </c>
@@ -1835,7 +1837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="39" t="s">
         <v>6</v>
       </c>
@@ -1898,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="39" t="s">
         <v>6</v>
       </c>
@@ -1961,7 +1963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="39" t="s">
         <v>6</v>
       </c>
@@ -2024,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="39" t="s">
         <v>6</v>
       </c>
@@ -2087,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="39" t="s">
         <v>6</v>
       </c>
@@ -2150,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="39" t="s">
         <v>6</v>
       </c>
@@ -2213,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="39" t="s">
         <v>6</v>
       </c>
@@ -2276,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="39" t="s">
         <v>6</v>
       </c>
@@ -2339,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="39" t="s">
         <v>6</v>
       </c>
@@ -2402,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="39" t="s">
         <v>6</v>
       </c>
@@ -2465,7 +2467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="39" t="s">
         <v>6</v>
       </c>
@@ -2528,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
         <v>6</v>
       </c>
@@ -2591,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="39" t="s">
         <v>6</v>
       </c>
@@ -2654,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
         <v>6</v>
       </c>
@@ -2717,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="39" t="s">
         <v>6</v>
       </c>
@@ -2780,7 +2782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="39" t="s">
         <v>6</v>
       </c>
@@ -2843,7 +2845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="39" t="s">
         <v>6</v>
       </c>
@@ -2906,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>6</v>
       </c>
@@ -2969,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="39" t="s">
         <v>6</v>
       </c>
@@ -3032,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="39" t="s">
         <v>6</v>
       </c>
@@ -3095,7 +3097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="39" t="s">
         <v>6</v>
       </c>
@@ -3158,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="39" t="s">
         <v>6</v>
       </c>
@@ -3221,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="39" t="s">
         <v>6</v>
       </c>
@@ -3301,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="39" t="s">
         <v>6</v>
       </c>
@@ -3364,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="39" t="s">
         <v>6</v>
       </c>
@@ -3427,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="39" t="s">
         <v>6</v>
       </c>
@@ -3490,7 +3492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="39" t="s">
         <v>6</v>
       </c>
@@ -3553,7 +3555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="39" t="s">
         <v>6</v>
       </c>
@@ -3616,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="39" t="s">
         <v>6</v>
       </c>
@@ -3679,7 +3681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="39" t="s">
         <v>6</v>
       </c>
@@ -3742,7 +3744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="40" t="s">
         <v>7</v>
       </c>
@@ -3805,7 +3807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="40" t="s">
         <v>7</v>
       </c>
@@ -3868,7 +3870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="40" t="s">
         <v>7</v>
       </c>
@@ -3931,7 +3933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="40" t="s">
         <v>7</v>
       </c>
@@ -3994,7 +3996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="40" t="s">
         <v>7</v>
       </c>
@@ -4057,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="40" t="s">
         <v>7</v>
       </c>
@@ -4120,7 +4122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="40" t="s">
         <v>7</v>
       </c>
@@ -4183,7 +4185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="40" t="s">
         <v>7</v>
       </c>
@@ -4246,7 +4248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="40" t="s">
         <v>7</v>
       </c>
@@ -4309,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="40" t="s">
         <v>7</v>
       </c>
@@ -4372,7 +4374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="40" t="s">
         <v>7</v>
       </c>
@@ -4435,7 +4437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="40" t="s">
         <v>7</v>
       </c>
@@ -4498,7 +4500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="40" t="s">
         <v>7</v>
       </c>
@@ -4561,7 +4563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="40" t="s">
         <v>7</v>
       </c>
@@ -4624,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="40" t="s">
         <v>7</v>
       </c>
@@ -4687,7 +4689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="40" t="s">
         <v>7</v>
       </c>
@@ -4750,7 +4752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="40" t="s">
         <v>7</v>
       </c>
@@ -4813,7 +4815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="40" t="s">
         <v>7</v>
       </c>
@@ -4876,7 +4878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="40" t="s">
         <v>7</v>
       </c>
@@ -4939,7 +4941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="40" t="s">
         <v>7</v>
       </c>
@@ -5002,7 +5004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="40" t="s">
         <v>7</v>
       </c>
@@ -5065,7 +5067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="40" t="s">
         <v>7</v>
       </c>
@@ -5128,7 +5130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="40" t="s">
         <v>7</v>
       </c>
@@ -5191,7 +5193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="40" t="s">
         <v>7</v>
       </c>
@@ -5254,7 +5256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="40" t="s">
         <v>7</v>
       </c>
@@ -5334,7 +5336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="40" t="s">
         <v>7</v>
       </c>
@@ -5397,7 +5399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="40" t="s">
         <v>7</v>
       </c>
@@ -5460,7 +5462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="40" t="s">
         <v>7</v>
       </c>
@@ -5523,7 +5525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="40" t="s">
         <v>7</v>
       </c>
@@ -5586,7 +5588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="40" t="s">
         <v>7</v>
       </c>
@@ -5649,7 +5651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="40" t="s">
         <v>7</v>
       </c>
@@ -5712,7 +5714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="40" t="s">
         <v>7</v>
       </c>
@@ -5827,24 +5829,24 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5" style="1" customWidth="1"/>
-    <col min="2" max="5" width="13.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="13.109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="24.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="1" customWidth="1"/>
     <col min="11" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="160" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="150.55000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -5885,7 +5887,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -5927,7 +5929,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -5969,7 +5971,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -6011,7 +6013,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -6053,7 +6055,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
@@ -6095,7 +6097,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -6137,7 +6139,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -6179,7 +6181,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
@@ -6221,7 +6223,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -6263,7 +6265,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
@@ -6305,7 +6307,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -6347,7 +6349,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -6389,7 +6391,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -6431,7 +6433,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -6473,7 +6475,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -6515,7 +6517,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -6557,7 +6559,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -6599,7 +6601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -6641,7 +6643,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
@@ -6683,7 +6685,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
@@ -6725,7 +6727,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -6767,7 +6769,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -6809,7 +6811,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -6851,7 +6853,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
@@ -6893,7 +6895,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
@@ -6935,7 +6937,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
@@ -6977,7 +6979,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
@@ -7019,7 +7021,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
@@ -7068,8 +7070,8 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7086,24 +7088,24 @@
       <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="14.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="2.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="2.109375" style="1" customWidth="1"/>
     <col min="4" max="5" width="14.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="2.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="2.109375" style="1" customWidth="1"/>
     <col min="7" max="8" width="14.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="2.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2.109375" style="1" customWidth="1"/>
     <col min="10" max="11" width="14.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="2.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="2.109375" style="1" customWidth="1"/>
     <col min="13" max="14" width="14.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="2.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="2.109375" style="1" customWidth="1"/>
     <col min="16" max="17" width="14.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="1"/>
+    <col min="18" max="18" width="10.77734375" customWidth="1"/>
+    <col min="19" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -7141,7 +7143,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -7183,7 +7185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -7224,7 +7226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -7241,12 +7243,12 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>